<commit_message>
fix some wrong dice values
</commit_message>
<xml_diff>
--- a/dice-analysis.xlsx
+++ b/dice-analysis.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Documents\mario-party-dice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CCA2EB-DC90-42F0-9AD7-3DA3C9812313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FB9E5C-9FB1-4A60-8857-D7961EC468E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{405F48AC-57AA-4B04-9495-3197A52998FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23797" windowHeight="13568" xr2:uid="{405F48AC-57AA-4B04-9495-3197A52998FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Mario</t>
   </si>
@@ -114,12 +113,6 @@
   </si>
   <si>
     <t>Std Dev of Dice</t>
-  </si>
-  <si>
-    <t>with Hammer Bro: x-intercept = 20.85</t>
-  </si>
-  <si>
-    <t>without Hammer Bro: x-intercept = 21.34</t>
   </si>
   <si>
     <t>Distance from point to line</t>
@@ -289,12 +282,12 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.13209689413823272"/>
-                  <c:y val="7.8138670166229218E-2"/>
+                  <c:x val="2.4653105861767281E-2"/>
+                  <c:y val="0.23844342373869934"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -836,7 +829,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,7 +1010,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,580 +1345,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Characters with coins on dice without Hammer Bro</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>(bubble size proportional to std dev of dice)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:bubbleChart>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$2:$L$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$M$2:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:bubbleSize>
-            <c:numRef>
-              <c:f>Sheet1!$N$2:$N$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0396078054371141</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.2776083947860748</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8989794855663558</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.4292856398964493</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1180339887498949</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4142135623730951</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5355339059327378</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:bubbleSize>
-          <c:bubble3D val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E681-47A9-9CA3-FB03DD859568}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:bubbleScale val="25"/>
-        <c:showNegBubbles val="0"/>
-        <c:axId val="441430032"/>
-        <c:axId val="441431672"/>
-      </c:bubbleChart>
-      <c:valAx>
-        <c:axId val="441430032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Total on Dice</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="441431672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="441431672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Total Coins</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="441430032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2031,10 +1450,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$10</c:f>
+              <c:f>Sheet1!$N$2:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2061,42 +1480,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9595917942265424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$10</c:f>
+              <c:f>Sheet1!$U$2:$U$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-0.76860204600729587</c:v>
+                  <c:v>-0.80244352485639159</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.2898360689845947</c:v>
+                  <c:v>-2.242105126471774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.46720946651637213</c:v>
+                  <c:v>-0.19101126866560628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.413179368144911</c:v>
+                  <c:v>2.6500536247003716</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.108050960225367</c:v>
+                  <c:v>1.261403102904709</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26639434309005822</c:v>
+                  <c:v>0.52244314716462081</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.30513025522305803</c:v>
+                  <c:v>-0.15275295880081463</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80665838073444318</c:v>
+                  <c:v>0.64997084671392391</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.76860204600729587</c:v>
+                  <c:v>-0.80244352485639159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.89171291454090285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2490,46 +1915,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3047,541 +2432,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4173,52 +3023,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>531018</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>215012</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>38098</xdr:rowOff>
+      <xdr:rowOff>43282</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
+      <xdr:colOff>336457</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1F19B89-5643-4AE7-BFBE-BDA07642FC82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>416718</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>88106</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>80963</xdr:rowOff>
+      <xdr:rowOff>36139</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4237,7 +3051,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4543,10 +3357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59E88C0-5668-4BAC-8200-A38B7D1A5014}">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AF35" sqref="AF35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4571,7 +3385,7 @@
         <v>25</v>
       </c>
       <c r="U1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.45">
@@ -4631,8 +3445,8 @@
         <v>6</v>
       </c>
       <c r="U2">
-        <f>(1.0795*L2+M2-23.039)/SQRT(1+1.0795*1.0795)</f>
-        <v>-0.76860204600729587</v>
+        <f>(1.0182*L2+M2-21.582)/SQRT(1+1.0182*1.0182)</f>
+        <v>-0.80244352485639159</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.45">
@@ -4695,8 +3509,8 @@
         <v>7</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U11" si="2">(1.0795*L3+M3-23.039)/SQRT(1+1.0795*1.0795)</f>
-        <v>-2.2898360689845947</v>
+        <f t="shared" ref="U3:U11" si="2">(1.0182*L3+M3-21.582)/SQRT(1+1.0182*1.0182)</f>
+        <v>-2.242105126471774</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.45">
@@ -4757,7 +3571,7 @@
       </c>
       <c r="U4">
         <f t="shared" si="2"/>
-        <v>-0.46720946651637213</v>
+        <v>-0.19101126866560628</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.45">
@@ -4821,7 +3635,7 @@
       </c>
       <c r="U5">
         <f t="shared" si="2"/>
-        <v>2.413179368144911</v>
+        <v>2.6500536247003716</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.45">
@@ -4885,7 +3699,7 @@
       </c>
       <c r="U6">
         <f t="shared" si="2"/>
-        <v>1.108050960225367</v>
+        <v>1.261403102904709</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
@@ -4946,7 +3760,7 @@
       </c>
       <c r="U7">
         <f t="shared" si="2"/>
-        <v>0.26639434309005822</v>
+        <v>0.52244314716462081</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
@@ -5010,7 +3824,7 @@
       </c>
       <c r="U8">
         <f t="shared" si="2"/>
-        <v>-0.30513025522305803</v>
+        <v>-0.15275295880081463</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
@@ -5071,7 +3885,7 @@
       </c>
       <c r="U9">
         <f t="shared" si="2"/>
-        <v>0.80665838073444318</v>
+        <v>0.64997084671392391</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
@@ -5132,7 +3946,7 @@
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>-0.76860204600729587</v>
+        <v>-0.80244352485639159</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
@@ -5170,7 +3984,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="M11">
         <v>3</v>
@@ -5186,13 +4000,17 @@
         <v>1</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R11">
         <v>5</v>
       </c>
       <c r="S11">
         <v>5</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="2"/>
+        <v>-0.89171291454090285</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
@@ -5224,14 +4042,6 @@
       <c r="I12">
         <f t="shared" si="4"/>
         <v>2.3570226039551585</v>
-      </c>
-    </row>
-    <row r="34" spans="12:21" x14ac:dyDescent="0.45">
-      <c r="L34" t="s">
-        <v>26</v>
-      </c>
-      <c r="U34" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up dice table, more on writeup
</commit_message>
<xml_diff>
--- a/dice-analysis.xlsx
+++ b/dice-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Documents\mario-party-dice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FB9E5C-9FB1-4A60-8857-D7961EC468E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38C1B14-6B63-4A83-A1C7-19C4B06026F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23797" windowHeight="13568" xr2:uid="{405F48AC-57AA-4B04-9495-3197A52998FE}"/>
   </bookViews>
@@ -3359,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59E88C0-5668-4BAC-8200-A38B7D1A5014}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>